<commit_message>
Working again - Lemma didn't help so much
</commit_message>
<xml_diff>
--- a/NaturalLanguageProcessing/QuestionAnsweringSystem/Results.xlsx
+++ b/NaturalLanguageProcessing/QuestionAnsweringSystem/Results.xlsx
@@ -12,9 +12,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="10140" windowHeight="8895"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="testset1" sheetId="1" r:id="rId1"/>
+    <sheet name="developset" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t>Current results</t>
   </si>
@@ -45,6 +47,108 @@
   </si>
   <si>
     <t>305/313</t>
+  </si>
+  <si>
+    <t>Who</t>
+  </si>
+  <si>
+    <t>What</t>
+  </si>
+  <si>
+    <t>When</t>
+  </si>
+  <si>
+    <t>Where</t>
+  </si>
+  <si>
+    <t>Why</t>
+  </si>
+  <si>
+    <t>How</t>
+  </si>
+  <si>
+    <t>which side</t>
+  </si>
+  <si>
+    <t>left side</t>
+  </si>
+  <si>
+    <t>on whom</t>
+  </si>
+  <si>
+    <t>on younger patients</t>
+  </si>
+  <si>
+    <t>whom did teach</t>
+  </si>
+  <si>
+    <t>apollo astronauts</t>
+  </si>
+  <si>
+    <t>Errors</t>
+  </si>
+  <si>
+    <t>for whom</t>
+  </si>
+  <si>
+    <t>people in europe</t>
+  </si>
+  <si>
+    <t>which provinces</t>
+  </si>
+  <si>
+    <t>british columbia, nova…</t>
+  </si>
+  <si>
+    <t>9-33-3</t>
+  </si>
+  <si>
+    <t>9-43-5</t>
+  </si>
+  <si>
+    <t>0-02-3</t>
+  </si>
+  <si>
+    <t>which towns</t>
+  </si>
+  <si>
+    <t>mainly small towns</t>
+  </si>
+  <si>
+    <t>from whom</t>
+  </si>
+  <si>
+    <t>the indian federal</t>
+  </si>
+  <si>
+    <t>0-05-4</t>
+  </si>
+  <si>
+    <t>0-06-5</t>
+  </si>
+  <si>
+    <t>whom does</t>
+  </si>
+  <si>
+    <t>six other climbers</t>
+  </si>
+  <si>
+    <t>Which</t>
+  </si>
+  <si>
+    <t>Whom</t>
+  </si>
+  <si>
+    <t>504/511</t>
+  </si>
+  <si>
+    <t>Getting rid of pronouns</t>
+  </si>
+  <si>
+    <t>Including all pronouns</t>
+  </si>
+  <si>
+    <t>Lemma</t>
   </si>
 </sst>
 </file>
@@ -60,12 +164,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -80,8 +190,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,16 +473,233 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G13" sqref="G13:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="4" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
   </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.40350000000000003</v>
+      </c>
+      <c r="C3">
+        <v>0.27529999999999999</v>
+      </c>
+      <c r="D3">
+        <v>0.32729999999999998</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>0.39340000000000003</v>
+      </c>
+      <c r="C14">
+        <v>0.2666</v>
+      </c>
+      <c r="D14">
+        <v>0.31780000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>0.38469999999999999</v>
+      </c>
+      <c r="C17">
+        <v>0.2676</v>
+      </c>
+      <c r="D17">
+        <v>0.31569999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>0.3851</v>
+      </c>
+      <c r="C20">
+        <v>0.27510000000000001</v>
+      </c>
+      <c r="D20">
+        <v>0.32100000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -397,16 +725,56 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.40350000000000003</v>
+        <v>0.42170000000000002</v>
       </c>
       <c r="C3">
-        <v>0.27529999999999999</v>
+        <v>0.28720000000000001</v>
       </c>
       <c r="D3">
-        <v>0.32729999999999998</v>
+        <v>0.3417</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>